<commit_message>
Updated the Test Case count
</commit_message>
<xml_diff>
--- a/Swag Labs/TestCase.xlsx
+++ b/Swag Labs/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Manual_Testing_Projects\Swag Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4434F4D6-0789-4EC3-AA36-06DAD75B01E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2904A378-E0EB-4EF2-B83D-7C3C46331E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40D7A449-F251-4F45-901B-A90AB279CD30}"/>
   </bookViews>
@@ -616,12 +616,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -651,6 +645,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -971,7 +971,7 @@
   <dimension ref="E2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,10 +982,10 @@
   <sheetData>
     <row r="2" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="5:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
@@ -1008,55 +1008,55 @@
         <v>4</v>
       </c>
       <c r="F6" s="6">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="10" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="18">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="18">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="24">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <f>SUM(F12:F15)</f>
         <v>20</v>
       </c>
@@ -1620,39 +1620,39 @@
       <c r="A5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>